<commit_message>
Add W3 mobile link to resources
</commit_message>
<xml_diff>
--- a/WCAG Guide for Tableau Dashboards v1.4.xlsx
+++ b/WCAG Guide for Tableau Dashboards v1.4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Parker\Documents\Clients\Alaska Department of Health\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hewinston\Documents\GitHub\AKDOHWCAG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4426E303-9E6F-4516-9740-E37126FFD780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B11DD8E-7E95-40DB-9F4D-C7B4CF67427C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{67E27043-D6D2-44B5-84F3-9AC46152F71C}"/>
+    <workbookView xWindow="28680" yWindow="-270" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{67E27043-D6D2-44B5-84F3-9AC46152F71C}"/>
   </bookViews>
   <sheets>
     <sheet name="Principles and Guidelines" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="401">
   <si>
     <t>Text Alternatives</t>
   </si>
@@ -1247,6 +1247,12 @@
   </si>
   <si>
     <t>Hours Estimate</t>
+  </si>
+  <si>
+    <t>Mobile Accessibility at W3C</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/WAI/standards-guidelines/mobile/</t>
   </si>
 </sst>
 </file>
@@ -1354,14 +1360,14 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
           <xfpb:DXFComplement i="0"/>
         </ext>
       </extLst>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1708,18 +1714,18 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{3D8A2720-AECF-4CC0-B22F-026C1EAFFF4D}" name="#" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{D1B2AD2F-D38D-4592-98FE-E4B96333A099}" name="Remediation" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{1BC43C37-DF53-4D31-A25F-F635556BDF4F}" name="Hours Estimate" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{2D8F622A-FA95-429F-9BF0-E5FE5AA30902}" name="Complete?" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{8B92EE67-C882-438A-9292-5D3BF805F4DF}" name="Example" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{58F5F2F6-C618-4D40-86AC-2E76FEC0E05C}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{1BC43C37-DF53-4D31-A25F-F635556BDF4F}" name="Hours Estimate" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{2D8F622A-FA95-429F-9BF0-E5FE5AA30902}" name="Complete?" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{8B92EE67-C882-438A-9292-5D3BF805F4DF}" name="Example" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{58F5F2F6-C618-4D40-86AC-2E76FEC0E05C}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{301E2472-55C8-4B3E-B131-BAD105ADE04E}" name="Table5" displayName="Table5" ref="A1:B11" totalsRowShown="0">
-  <autoFilter ref="A1:B11" xr:uid="{301E2472-55C8-4B3E-B131-BAD105ADE04E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{301E2472-55C8-4B3E-B131-BAD105ADE04E}" name="Table5" displayName="Table5" ref="A1:B12" totalsRowShown="0">
+  <autoFilter ref="A1:B12" xr:uid="{301E2472-55C8-4B3E-B131-BAD105ADE04E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B10">
     <sortCondition descending="1" ref="B1:B10"/>
   </sortState>
@@ -2054,16 +2060,16 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.86328125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="49.1328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="153.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1328125" style="2"/>
+    <col min="1" max="1" width="6.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="49.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="153.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -2074,7 +2080,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2085,7 +2091,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2096,7 +2102,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2107,7 +2113,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2118,7 +2124,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>142</v>
       </c>
@@ -2129,7 +2135,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -2140,7 +2146,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1.2</v>
       </c>
@@ -2151,7 +2157,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1.3</v>
       </c>
@@ -2162,7 +2168,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1.4</v>
       </c>
@@ -2173,7 +2179,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2.1</v>
       </c>
@@ -2184,7 +2190,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>2.2000000000000002</v>
       </c>
@@ -2195,7 +2201,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>2.2999999999999998</v>
       </c>
@@ -2206,7 +2212,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>2.4</v>
       </c>
@@ -2217,7 +2223,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>2.5</v>
       </c>
@@ -2228,7 +2234,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>3.1</v>
       </c>
@@ -2239,7 +2245,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>3.2</v>
       </c>
@@ -2250,7 +2256,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>3.3</v>
       </c>
@@ -2261,7 +2267,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>4.0999999999999996</v>
       </c>
@@ -2272,7 +2278,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>142</v>
       </c>
@@ -2283,7 +2289,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>1</v>
       </c>
@@ -2294,7 +2300,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>2</v>
       </c>
@@ -2305,7 +2311,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>3</v>
       </c>
@@ -2334,25 +2340,25 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.265625" customWidth="1"/>
-    <col min="4" max="4" width="29.86328125" customWidth="1"/>
-    <col min="5" max="5" width="8.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.1328125" customWidth="1"/>
-    <col min="7" max="7" width="41.265625" customWidth="1"/>
-    <col min="8" max="8" width="24.59765625" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" customWidth="1"/>
+    <col min="7" max="7" width="41.28515625" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" customWidth="1"/>
     <col min="9" max="10" width="39" customWidth="1"/>
-    <col min="11" max="11" width="106.86328125" customWidth="1"/>
-    <col min="12" max="13" width="255.73046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.1328125" customWidth="1"/>
-    <col min="15" max="15" width="255.73046875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="49.3984375" customWidth="1"/>
+    <col min="11" max="11" width="106.85546875" customWidth="1"/>
+    <col min="12" max="13" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" customWidth="1"/>
+    <col min="15" max="15" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>236</v>
       </c>
@@ -2381,7 +2387,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -2410,7 +2416,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8" t="s">
         <v>311</v>
@@ -2435,7 +2441,7 @@
       </c>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="8" t="s">
         <v>312</v>
@@ -2460,7 +2466,7 @@
       </c>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8" t="s">
         <v>313</v>
@@ -2485,7 +2491,7 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8" t="s">
         <v>314</v>
@@ -2510,7 +2516,7 @@
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8" t="s">
         <v>315</v>
@@ -2535,7 +2541,7 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8" t="s">
         <v>306</v>
@@ -2560,7 +2566,7 @@
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8" t="s">
         <v>307</v>
@@ -2585,7 +2591,7 @@
       </c>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8" t="s">
         <v>308</v>
@@ -2610,7 +2616,7 @@
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8" t="s">
         <v>309</v>
@@ -2635,7 +2641,7 @@
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>2</v>
       </c>
@@ -2664,7 +2670,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>3</v>
       </c>
@@ -2693,7 +2699,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>4</v>
       </c>
@@ -2722,7 +2728,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>5</v>
       </c>
@@ -2751,7 +2757,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8" t="s">
         <v>317</v>
@@ -2776,7 +2782,7 @@
       </c>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8" t="s">
         <v>318</v>
@@ -2801,7 +2807,7 @@
       </c>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>6</v>
       </c>
@@ -2830,7 +2836,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8" t="s">
         <v>319</v>
@@ -2855,7 +2861,7 @@
       </c>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>7</v>
       </c>
@@ -2884,7 +2890,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>8</v>
       </c>
@@ -2913,7 +2919,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8" t="s">
         <v>322</v>
@@ -2938,7 +2944,7 @@
       </c>
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8" t="s">
         <v>323</v>
@@ -2963,7 +2969,7 @@
       </c>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="8" t="s">
         <v>324</v>
@@ -2988,7 +2994,7 @@
       </c>
       <c r="I24" s="6"/>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8" t="s">
         <v>325</v>
@@ -3013,7 +3019,7 @@
       </c>
       <c r="I25" s="6"/>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8" t="s">
         <v>326</v>
@@ -3038,7 +3044,7 @@
       </c>
       <c r="I26" s="6"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>9</v>
       </c>
@@ -3067,7 +3073,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>10</v>
       </c>
@@ -3096,7 +3102,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="8" t="s">
         <v>130</v>
@@ -3121,7 +3127,7 @@
       </c>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>11</v>
       </c>
@@ -3150,7 +3156,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8" t="s">
         <v>327</v>
@@ -3175,7 +3181,7 @@
       </c>
       <c r="I31" s="6"/>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8" t="s">
         <v>328</v>
@@ -3200,7 +3206,7 @@
       </c>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="8" t="s">
         <v>329</v>
@@ -3225,7 +3231,7 @@
       </c>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="8" t="s">
         <v>330</v>
@@ -3250,7 +3256,7 @@
       </c>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8" t="s">
         <v>331</v>
@@ -3275,7 +3281,7 @@
       </c>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8" t="s">
         <v>332</v>
@@ -3300,7 +3306,7 @@
       </c>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8" t="s">
         <v>333</v>
@@ -3325,7 +3331,7 @@
       </c>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="8" t="s">
         <v>334</v>
@@ -3350,7 +3356,7 @@
       </c>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="8" t="s">
         <v>335</v>
@@ -3375,7 +3381,7 @@
       </c>
       <c r="I39" s="6"/>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="8" t="s">
         <v>336</v>
@@ -3400,7 +3406,7 @@
       </c>
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="8" t="s">
         <v>337</v>
@@ -3425,7 +3431,7 @@
       </c>
       <c r="I41" s="6"/>
     </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="8" t="s">
         <v>338</v>
@@ -3450,7 +3456,7 @@
       </c>
       <c r="I42" s="6"/>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="8" t="s">
         <v>339</v>
@@ -3475,7 +3481,7 @@
       </c>
       <c r="I43" s="6"/>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="8" t="s">
         <v>340</v>
@@ -3500,7 +3506,7 @@
       </c>
       <c r="I44" s="6"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>12</v>
       </c>
@@ -3529,7 +3535,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="8" t="s">
         <v>341</v>
@@ -3554,7 +3560,7 @@
       </c>
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>13</v>
       </c>
@@ -3583,7 +3589,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>14</v>
       </c>
@@ -3612,7 +3618,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>15</v>
       </c>
@@ -3641,7 +3647,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>16</v>
       </c>
@@ -3670,7 +3676,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="8" t="s">
         <v>346</v>
@@ -3695,7 +3701,7 @@
       </c>
       <c r="I51" s="6"/>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="8" t="s">
         <v>347</v>
@@ -3720,7 +3726,7 @@
       </c>
       <c r="I52" s="6"/>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="8" t="s">
         <v>168</v>
@@ -3745,7 +3751,7 @@
       </c>
       <c r="I53" s="6"/>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="8" t="s">
         <v>170</v>
@@ -3770,7 +3776,7 @@
       </c>
       <c r="I54" s="6"/>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="8" t="s">
         <v>172</v>
@@ -3795,7 +3801,7 @@
       </c>
       <c r="I55" s="6"/>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="8" t="s">
         <v>174</v>
@@ -3820,7 +3826,7 @@
       </c>
       <c r="I56" s="6"/>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="8" t="s">
         <v>348</v>
@@ -3845,7 +3851,7 @@
       </c>
       <c r="I57" s="6"/>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="8" t="s">
         <v>349</v>
@@ -3870,7 +3876,7 @@
       </c>
       <c r="I58" s="6"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>17</v>
       </c>
@@ -3899,7 +3905,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="8" t="s">
         <v>351</v>
@@ -3924,7 +3930,7 @@
       </c>
       <c r="I60" s="6"/>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="8" t="s">
         <v>352</v>
@@ -3949,7 +3955,7 @@
       </c>
       <c r="I61" s="6"/>
     </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="8" t="s">
         <v>353</v>
@@ -3974,7 +3980,7 @@
       </c>
       <c r="I62" s="6"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>18</v>
       </c>
@@ -4003,7 +4009,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>19</v>
       </c>
@@ -4032,7 +4038,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>20</v>
       </c>
@@ -4061,7 +4067,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="8">
         <v>21</v>
       </c>
@@ -4090,7 +4096,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="8" t="s">
         <v>358</v>
@@ -4115,7 +4121,7 @@
       </c>
       <c r="I67" s="6"/>
     </row>
-    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="8" t="s">
         <v>359</v>
@@ -4140,7 +4146,7 @@
       </c>
       <c r="I68" s="6"/>
     </row>
-    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="8" t="s">
         <v>360</v>
@@ -4165,7 +4171,7 @@
       </c>
       <c r="I69" s="6"/>
     </row>
-    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="8" t="s">
         <v>361</v>
@@ -4190,7 +4196,7 @@
       </c>
       <c r="I70" s="6"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <v>22</v>
       </c>
@@ -4219,7 +4225,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <v>23</v>
       </c>
@@ -4248,7 +4254,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <v>24</v>
       </c>
@@ -4277,7 +4283,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <v>25</v>
       </c>
@@ -4306,7 +4312,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="8"/>
       <c r="B75" s="8" t="s">
         <v>366</v>
@@ -4331,7 +4337,7 @@
       </c>
       <c r="I75" s="6"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <v>26</v>
       </c>
@@ -4360,7 +4366,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <v>27</v>
       </c>
@@ -4389,7 +4395,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <v>28</v>
       </c>
@@ -4418,7 +4424,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <v>29</v>
       </c>
@@ -4447,7 +4453,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="8" t="s">
         <v>371</v>
@@ -4472,7 +4478,7 @@
       </c>
       <c r="I80" s="6"/>
     </row>
-    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
       <c r="B81" s="8" t="s">
         <v>372</v>
@@ -4497,7 +4503,7 @@
       </c>
       <c r="I81" s="6"/>
     </row>
-    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="8"/>
       <c r="B82" s="8" t="s">
         <v>373</v>
@@ -4522,7 +4528,7 @@
       </c>
       <c r="I82" s="6"/>
     </row>
-    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="8"/>
       <c r="B83" s="8" t="s">
         <v>374</v>
@@ -4547,7 +4553,7 @@
       </c>
       <c r="I83" s="6"/>
     </row>
-    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="B84" s="8" t="s">
         <v>375</v>
@@ -4572,7 +4578,7 @@
       </c>
       <c r="I84" s="6"/>
     </row>
-    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="8"/>
       <c r="B85" s="8" t="s">
         <v>376</v>
@@ -4597,7 +4603,7 @@
       </c>
       <c r="I85" s="6"/>
     </row>
-    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="8"/>
       <c r="B86" s="8" t="s">
         <v>377</v>
@@ -4622,7 +4628,7 @@
       </c>
       <c r="I86" s="6"/>
     </row>
-    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="8"/>
       <c r="B87" s="8" t="s">
         <v>378</v>
@@ -4647,7 +4653,7 @@
       </c>
       <c r="I87" s="6"/>
     </row>
-    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
       <c r="B88" s="8" t="s">
         <v>379</v>
@@ -4686,20 +4692,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D533DA-9B44-4E62-8880-E2761E1543A9}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="123.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.73046875" customWidth="1"/>
-    <col min="4" max="4" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="114.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="123.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="114.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>142</v>
       </c>
@@ -4719,7 +4725,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>301</v>
       </c>
@@ -4739,7 +4745,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>302</v>
       </c>
@@ -4757,7 +4763,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>303</v>
       </c>
@@ -4773,7 +4779,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>304</v>
       </c>
@@ -4789,7 +4795,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>305</v>
       </c>
@@ -4805,7 +4811,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>310</v>
       </c>
@@ -4821,7 +4827,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>342</v>
       </c>
@@ -4837,7 +4843,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>350</v>
       </c>
@@ -4853,7 +4859,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>356</v>
       </c>
@@ -4869,7 +4875,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>362</v>
       </c>
@@ -4885,7 +4891,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>363</v>
       </c>
@@ -4901,7 +4907,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>367</v>
       </c>
@@ -4917,7 +4923,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>368</v>
       </c>
@@ -4935,7 +4941,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>369</v>
       </c>
@@ -4951,7 +4957,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>316</v>
       </c>
@@ -4969,7 +4975,7 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>128</v>
       </c>
@@ -4985,7 +4991,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>129</v>
       </c>
@@ -5001,7 +5007,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>131</v>
       </c>
@@ -5017,7 +5023,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>320</v>
       </c>
@@ -5033,7 +5039,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>321</v>
       </c>
@@ -5049,7 +5055,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>343</v>
       </c>
@@ -5065,7 +5071,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>344</v>
       </c>
@@ -5081,7 +5087,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>345</v>
       </c>
@@ -5097,7 +5103,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>354</v>
       </c>
@@ -5113,7 +5119,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>355</v>
       </c>
@@ -5129,7 +5135,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>357</v>
       </c>
@@ -5145,7 +5151,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>364</v>
       </c>
@@ -5161,7 +5167,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>365</v>
       </c>
@@ -5177,7 +5183,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>370</v>
       </c>
@@ -5205,19 +5211,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FBDB377-5604-4EAA-9070-5106CD4944D3}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="83.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="77.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="83.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>380</v>
       </c>
@@ -5225,7 +5231,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>387</v>
       </c>
@@ -5233,7 +5239,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>388</v>
       </c>
@@ -5241,7 +5247,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>385</v>
       </c>
@@ -5249,7 +5255,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>389</v>
       </c>
@@ -5257,7 +5263,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>295</v>
       </c>
@@ -5265,7 +5271,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>390</v>
       </c>
@@ -5273,7 +5279,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>393</v>
       </c>
@@ -5281,7 +5287,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>391</v>
       </c>
@@ -5289,7 +5295,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>392</v>
       </c>
@@ -5297,12 +5303,20 @@
         <v>383</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>394</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>384</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>399</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small correction to guidelines 2.1.01 and 2.1.03
</commit_message>
<xml_diff>
--- a/WCAG Guide for Tableau Dashboards v1.4.xlsx
+++ b/WCAG Guide for Tableau Dashboards v1.4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hewinston\Documents\GitHub\AKDOHWCAG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\HSSJNUVSSFP2\Share1\SHARED\Juneau-Research\Training Binder\Accessibility\WCAG Guides\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B11DD8E-7E95-40DB-9F4D-C7B4CF67427C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC63D7BD-0CE8-48C9-ABB8-6FCC47DF30BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-270" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{67E27043-D6D2-44B5-84F3-9AC46152F71C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{67E27043-D6D2-44B5-84F3-9AC46152F71C}"/>
   </bookViews>
   <sheets>
     <sheet name="Principles and Guidelines" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="400">
   <si>
     <t>Text Alternatives</t>
   </si>
@@ -1246,13 +1246,10 @@
     <t>Does the default alt text serve the same purpose as the graph?</t>
   </si>
   <si>
-    <t>Hours Estimate</t>
+    <t>https://www.w3.org/WAI/standards-guidelines/mobile/</t>
   </si>
   <si>
     <t>Mobile Accessibility at W3C</t>
-  </si>
-  <si>
-    <t>https://www.w3.org/WAI/standards-guidelines/mobile/</t>
   </si>
 </sst>
 </file>
@@ -1354,7 +1351,7 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="31">
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1365,9 +1362,6 @@
           <xfpb:DXFComplement i="0"/>
         </ext>
       </extLst>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1646,75 +1640,74 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2C6E20B6-50CE-498C-A79A-9FE717A1D4B6}" name="Table2" displayName="Table2" ref="A1:C5" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2C6E20B6-50CE-498C-A79A-9FE717A1D4B6}" name="Table2" displayName="Table2" ref="A1:C5" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="A1:C5" xr:uid="{2C6E20B6-50CE-498C-A79A-9FE717A1D4B6}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3005B307-DB81-46DE-B366-2DE090774535}" name="#" dataDxfId="29" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{7386C8B5-4B7A-4BF0-B86F-AEBB8576CC2E}" name="Principals" dataDxfId="28" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{003C34D6-6979-4E32-A103-D2BAB30A1B25}" name="Description" dataDxfId="27" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{3005B307-DB81-46DE-B366-2DE090774535}" name="#" dataDxfId="28" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{7386C8B5-4B7A-4BF0-B86F-AEBB8576CC2E}" name="Principals" dataDxfId="27" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{003C34D6-6979-4E32-A103-D2BAB30A1B25}" name="Description" dataDxfId="26" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{67D84F09-2FAF-4B89-A276-1E384E66FE7E}" name="Table3" displayName="Table3" ref="A7:C20" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{67D84F09-2FAF-4B89-A276-1E384E66FE7E}" name="Table3" displayName="Table3" ref="A7:C20" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="A7:C20" xr:uid="{67D84F09-2FAF-4B89-A276-1E384E66FE7E}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{CD9C37F7-9172-4C23-B229-8606D9325D5D}" name="#" dataDxfId="24" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{CF1C6F75-CB81-493D-8FD4-63706055BE4E}" name="Guidelines" dataDxfId="23" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{BAF190EC-5E45-4C96-A340-BB7377F9E9B1}" name="Description" dataDxfId="22" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{CD9C37F7-9172-4C23-B229-8606D9325D5D}" name="#" dataDxfId="23" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{CF1C6F75-CB81-493D-8FD4-63706055BE4E}" name="Guidelines" dataDxfId="22" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{BAF190EC-5E45-4C96-A340-BB7377F9E9B1}" name="Description" dataDxfId="21" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{65A04FF3-DCB4-4C2C-B339-8AC4317B6575}" name="Table4" displayName="Table4" ref="A22:C25" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{65A04FF3-DCB4-4C2C-B339-8AC4317B6575}" name="Table4" displayName="Table4" ref="A22:C25" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A22:C25" xr:uid="{65A04FF3-DCB4-4C2C-B339-8AC4317B6575}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F01449D5-A4B5-471F-8266-EB72FC93AA4E}" name="#" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{9F67E405-C80D-4057-BEF0-B9AC18C0D160}" name="Level" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{A3F114AF-2AF1-4CC1-9CD5-3F8F5C9E8928}" name="Description" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{F01449D5-A4B5-471F-8266-EB72FC93AA4E}" name="#" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{9F67E405-C80D-4057-BEF0-B9AC18C0D160}" name="Level" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{A3F114AF-2AF1-4CC1-9CD5-3F8F5C9E8928}" name="Description" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A310025-931B-4D2D-B3C3-0A29936F8E75}" name="wcag_csv_1" displayName="wcag_csv_1" ref="A1:I88" tableType="queryTable" totalsRowShown="0" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A310025-931B-4D2D-B3C3-0A29936F8E75}" name="wcag_csv_1" displayName="wcag_csv_1" ref="A1:I88" tableType="queryTable" totalsRowShown="0" dataDxfId="15">
   <autoFilter ref="A1:I88" xr:uid="{5A310025-931B-4D2D-B3C3-0A29936F8E75}">
     <filterColumn colId="7">
       <filters>
-        <filter val="Yes"/>
+        <filter val="NA"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I79">
-    <sortCondition ref="A1:A88"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I88">
+    <sortCondition ref="E1:E88"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="11" xr3:uid="{99B3D30B-38F3-442F-95D6-0D80332A53D2}" uniqueName="11" name="Order" queryTableFieldId="30" dataDxfId="15" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{7D52A57B-AC7E-40ED-A5E1-04EAB573E76E}" uniqueName="12" name="#" queryTableFieldId="31" dataDxfId="14" dataCellStyle="Comma"/>
-    <tableColumn id="5" xr3:uid="{9FB6F907-7EFA-48BD-8E0F-24B6B0A1CD25}" uniqueName="5" name="Principal" queryTableFieldId="5" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{5368A4B1-2745-482F-8E9A-1BF7D8F4A218}" uniqueName="2" name="Guideline" queryTableFieldId="2" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{FAA49593-0176-487A-8B7B-A26890E726BE}" uniqueName="3" name="Level" queryTableFieldId="3" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{4AA4A539-352E-46CA-945D-A64B76D5125D}" uniqueName="10" name="Criteria" queryTableFieldId="13" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{677C5527-9766-45FE-8431-F54AB7CBBA10}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{59E324A2-D411-450B-9DD6-6E7380B5A450}" uniqueName="6" name="Remediable in Tableau? (Yes, No, NA)" queryTableFieldId="25" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{DA59A024-D85F-49E2-B4A8-397D73149BB1}" uniqueName="8" name="If So, How?" queryTableFieldId="29" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{99B3D30B-38F3-442F-95D6-0D80332A53D2}" uniqueName="11" name="Order" queryTableFieldId="30" dataDxfId="14" dataCellStyle="Comma"/>
+    <tableColumn id="12" xr3:uid="{7D52A57B-AC7E-40ED-A5E1-04EAB573E76E}" uniqueName="12" name="#" queryTableFieldId="31" dataDxfId="13" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{9FB6F907-7EFA-48BD-8E0F-24B6B0A1CD25}" uniqueName="5" name="Principal" queryTableFieldId="5" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{5368A4B1-2745-482F-8E9A-1BF7D8F4A218}" uniqueName="2" name="Guideline" queryTableFieldId="2" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{FAA49593-0176-487A-8B7B-A26890E726BE}" uniqueName="3" name="Level" queryTableFieldId="3" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{4AA4A539-352E-46CA-945D-A64B76D5125D}" uniqueName="10" name="Criteria" queryTableFieldId="13" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{677C5527-9766-45FE-8431-F54AB7CBBA10}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{59E324A2-D411-450B-9DD6-6E7380B5A450}" uniqueName="6" name="Remediable in Tableau? (Yes, No, NA)" queryTableFieldId="25" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{DA59A024-D85F-49E2-B4A8-397D73149BB1}" uniqueName="8" name="If So, How?" queryTableFieldId="29" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{86977D78-0EC5-431A-942E-7AA246ABADC5}" name="Table58" displayName="Table58" ref="A1:F30" totalsRowShown="0" dataDxfId="6">
-  <autoFilter ref="A1:F30" xr:uid="{86977D78-0EC5-431A-942E-7AA246ABADC5}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{3D8A2720-AECF-4CC0-B22F-026C1EAFFF4D}" name="#" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{D1B2AD2F-D38D-4592-98FE-E4B96333A099}" name="Remediation" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{1BC43C37-DF53-4D31-A25F-F635556BDF4F}" name="Hours Estimate" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{86977D78-0EC5-431A-942E-7AA246ABADC5}" name="Table58" displayName="Table58" ref="A1:E30" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E30" xr:uid="{86977D78-0EC5-431A-942E-7AA246ABADC5}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{3D8A2720-AECF-4CC0-B22F-026C1EAFFF4D}" name="#" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{D1B2AD2F-D38D-4592-98FE-E4B96333A099}" name="Remediation" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{2D8F622A-FA95-429F-9BF0-E5FE5AA30902}" name="Complete?" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{8B92EE67-C882-438A-9292-5D3BF805F4DF}" name="Example" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{58F5F2F6-C618-4D40-86AC-2E76FEC0E05C}" name="Notes" dataDxfId="0"/>
@@ -2336,8 +2329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D585E9-5828-430F-BD2A-15125DCCC36B}">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2387,7 +2380,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -2416,7 +2409,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8" t="s">
         <v>311</v>
@@ -2441,7 +2434,7 @@
       </c>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="8" t="s">
         <v>312</v>
@@ -2466,7 +2459,7 @@
       </c>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8" t="s">
         <v>313</v>
@@ -2492,315 +2485,339 @@
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="8">
+        <v>2</v>
+      </c>
       <c r="B6" s="8" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I6" s="6"/>
+        <v>232</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="8">
+        <v>3</v>
+      </c>
       <c r="B7" s="8" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I7" s="6"/>
+        <v>232</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="8">
+        <v>4</v>
+      </c>
       <c r="B8" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I8" s="6"/>
+        <v>232</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="A9" s="8">
+        <v>5</v>
+      </c>
       <c r="B9" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I9" s="6"/>
+        <v>232</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="A10" s="8">
+        <v>6</v>
+      </c>
       <c r="B10" s="8" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>119</v>
+        <v>159</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>302</v>
+        <v>342</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>121</v>
+        <v>161</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>232</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>303</v>
+        <v>350</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>122</v>
+        <v>177</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>232</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>304</v>
+        <v>356</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>123</v>
+        <v>183</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="I14" s="6" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" s="9" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
+        <v>10</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>2</v>
-      </c>
       <c r="D15" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>127</v>
+        <v>189</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>232</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+      <c r="A16" s="8">
+        <v>11</v>
+      </c>
       <c r="B16" s="8" t="s">
-        <v>317</v>
+        <v>363</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>125</v>
+        <v>190</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>235</v>
@@ -2808,53 +2825,49 @@
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>6</v>
-      </c>
+      <c r="A18" s="8"/>
       <c r="B18" s="8" t="s">
-        <v>310</v>
+        <v>327</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8" t="s">
-        <v>319</v>
+        <v>330</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>235</v>
@@ -2862,107 +2875,99 @@
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
-        <v>7</v>
-      </c>
+      <c r="A20" s="8"/>
       <c r="B20" s="8" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>243</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
-        <v>8</v>
-      </c>
+      <c r="A21" s="8"/>
       <c r="B21" s="8" t="s">
-        <v>350</v>
+        <v>332</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8" t="s">
-        <v>322</v>
+        <v>337</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8" t="s">
-        <v>323</v>
+        <v>340</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>235</v>
@@ -2970,49 +2975,53 @@
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="A24" s="8">
+        <v>12</v>
+      </c>
       <c r="B24" s="8" t="s">
-        <v>324</v>
+        <v>367</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>141</v>
+        <v>194</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I24" s="6"/>
-    </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8" t="s">
-        <v>325</v>
+        <v>341</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>235</v>
@@ -3020,107 +3029,107 @@
       <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+      <c r="A26" s="8">
+        <v>13</v>
+      </c>
       <c r="B26" s="8" t="s">
-        <v>326</v>
+        <v>368</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I26" s="6"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>356</v>
+        <v>369</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>245</v>
+      <c r="I27" s="6" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
-        <v>10</v>
-      </c>
+      <c r="A28" s="8"/>
       <c r="B28" s="8" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="8" t="s">
-        <v>130</v>
+        <v>349</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>139</v>
+        <v>176</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>235</v>
@@ -3128,228 +3137,224 @@
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
-        <v>11</v>
-      </c>
+      <c r="A30" s="8"/>
       <c r="B30" s="8" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8" t="s">
-        <v>327</v>
+        <v>374</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>146</v>
+        <v>201</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I31" s="6"/>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8" t="s">
-        <v>328</v>
+        <v>377</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>148</v>
+        <v>206</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="H32" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="8" t="s">
-        <v>329</v>
+        <v>378</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>145</v>
+        <v>204</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="H33" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="8" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>92</v>
+        <v>24</v>
       </c>
       <c r="H34" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>149</v>
+        <v>116</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="H36" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="H37" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="8" t="s">
-        <v>334</v>
+        <v>130</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>43</v>
+        <v>102</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>235</v>
@@ -3357,74 +3362,82 @@
       <c r="I38" s="6"/>
     </row>
     <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
+      <c r="A39" s="8">
+        <v>15</v>
+      </c>
       <c r="B39" s="8" t="s">
-        <v>335</v>
+        <v>316</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I39" s="6"/>
+        <v>232</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
+      <c r="A40" s="8">
+        <v>16</v>
+      </c>
       <c r="B40" s="8" t="s">
-        <v>336</v>
+        <v>128</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I40" s="6"/>
-    </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="8" t="s">
-        <v>337</v>
+        <v>170</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="H41" s="6" t="s">
         <v>235</v>
@@ -3432,113 +3445,127 @@
       <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
+      <c r="A42" s="8">
+        <v>17</v>
+      </c>
       <c r="B42" s="8" t="s">
-        <v>338</v>
+        <v>129</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I42" s="6"/>
+        <v>232</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
+      <c r="A43" s="8">
+        <v>18</v>
+      </c>
       <c r="B43" s="8" t="s">
-        <v>339</v>
+        <v>131</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I43" s="6"/>
+        <v>232</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
+      <c r="A44" s="8">
+        <v>19</v>
+      </c>
       <c r="B44" s="8" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I44" s="6"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>367</v>
+        <v>321</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>194</v>
+        <v>134</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>109</v>
+        <v>37</v>
       </c>
       <c r="H45" s="6" t="s">
         <v>232</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
     </row>
     <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="8"/>
+      <c r="A46" s="8">
+        <v>21</v>
+      </c>
       <c r="B46" s="8" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>4</v>
@@ -3547,329 +3574,347 @@
         <v>14</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I46" s="6"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>195</v>
+        <v>163</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>232</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
+        <v>23</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="8" t="s">
-        <v>369</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="E48" s="6" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>196</v>
+        <v>164</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="H48" s="6" t="s">
         <v>232</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
+        <v>24</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>124</v>
+        <v>181</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="H49" s="6" t="s">
         <v>232</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>128</v>
+        <v>355</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>137</v>
+        <v>182</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="H50" s="6" t="s">
         <v>232</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="8"/>
+      <c r="A51" s="8">
+        <v>26</v>
+      </c>
       <c r="B51" s="8" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I51" s="6"/>
+        <v>232</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="8"/>
+      <c r="A52" s="8">
+        <v>27</v>
+      </c>
       <c r="B52" s="8" t="s">
-        <v>347</v>
+        <v>364</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>166</v>
+        <v>191</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I52" s="6"/>
+        <v>232</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="8"/>
+      <c r="A53" s="8">
+        <v>28</v>
+      </c>
       <c r="B53" s="8" t="s">
-        <v>168</v>
+        <v>365</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>167</v>
+        <v>192</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I53" s="6"/>
+        <v>232</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="8"/>
+      <c r="A54" s="8">
+        <v>29</v>
+      </c>
       <c r="B54" s="8" t="s">
-        <v>170</v>
+        <v>370</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>169</v>
+        <v>197</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I54" s="6"/>
-    </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="8" t="s">
-        <v>172</v>
+        <v>371</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>171</v>
+        <v>198</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>60</v>
+        <v>395</v>
       </c>
       <c r="H55" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I55" s="6"/>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="8" t="s">
-        <v>174</v>
+        <v>375</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>173</v>
+        <v>202</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I56" s="6"/>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="8" t="s">
-        <v>348</v>
+        <v>379</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>175</v>
+        <v>205</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="H57" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I57" s="6"/>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="8" t="s">
-        <v>349</v>
+        <v>306</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>176</v>
+        <v>117</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>235</v>
@@ -3877,103 +3922,99 @@
       <c r="I58" s="6"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="8">
-        <v>17</v>
-      </c>
+      <c r="A59" s="8"/>
       <c r="B59" s="8" t="s">
-        <v>129</v>
+        <v>307</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I59" s="6" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="I59" s="6"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="8" t="s">
-        <v>351</v>
+        <v>308</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>178</v>
+        <v>119</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>89</v>
+        <v>28</v>
       </c>
       <c r="H60" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I60" s="6"/>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="8" t="s">
-        <v>352</v>
+        <v>309</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>179</v>
+        <v>120</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>90</v>
+        <v>29</v>
       </c>
       <c r="H61" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I61" s="6"/>
     </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="8" t="s">
-        <v>353</v>
+        <v>318</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>180</v>
+        <v>126</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="H62" s="6" t="s">
         <v>235</v>
@@ -3981,11 +4022,9 @@
       <c r="I62" s="6"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="8">
-        <v>18</v>
-      </c>
+      <c r="A63" s="8"/>
       <c r="B63" s="8" t="s">
-        <v>131</v>
+        <v>323</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>2</v>
@@ -3994,27 +4033,23 @@
         <v>10</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I63" s="6" t="s">
-        <v>253</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="I63" s="6"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="8">
-        <v>19</v>
-      </c>
+      <c r="A64" s="8"/>
       <c r="B64" s="8" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>2</v>
@@ -4023,27 +4058,23 @@
         <v>10</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I64" s="6" t="s">
-        <v>254</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="I64" s="6"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="8">
-        <v>20</v>
-      </c>
+      <c r="A65" s="8"/>
       <c r="B65" s="8" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>2</v>
@@ -4052,144 +4083,138 @@
         <v>10</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I65" s="6" t="s">
-        <v>255</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="I65" s="6"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="8">
+      <c r="A66" s="8"/>
+      <c r="B66" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B66" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>20</v>
-      </c>
       <c r="F66" s="6" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I66" s="6" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="I66" s="6"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="8" t="s">
-        <v>358</v>
+        <v>329</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>185</v>
+        <v>145</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="H67" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I67" s="6"/>
     </row>
-    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="8" t="s">
-        <v>359</v>
+        <v>333</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="H68" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I68" s="6"/>
     </row>
-    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="8" t="s">
-        <v>360</v>
+        <v>334</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>187</v>
+        <v>152</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="H69" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I69" s="6"/>
     </row>
-    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="8" t="s">
-        <v>361</v>
+        <v>335</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="H70" s="6" t="s">
         <v>235</v>
@@ -4197,140 +4222,124 @@
       <c r="I70" s="6"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="8">
-        <v>22</v>
-      </c>
+      <c r="A71" s="8"/>
       <c r="B71" s="8" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I71" s="6" t="s">
-        <v>262</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="I71" s="6"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="8">
-        <v>23</v>
-      </c>
+      <c r="A72" s="8"/>
       <c r="B72" s="8" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I72" s="6" t="s">
-        <v>257</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="I72" s="6"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="8">
-        <v>24</v>
-      </c>
+      <c r="A73" s="8"/>
       <c r="B73" s="8" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I73" s="6" t="s">
-        <v>258</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="I73" s="6"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="8">
-        <v>25</v>
-      </c>
+      <c r="A74" s="8"/>
       <c r="B74" s="8" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I74" s="6" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="I74" s="6"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="8"/>
       <c r="B75" s="8" t="s">
-        <v>366</v>
+        <v>347</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="H75" s="6" t="s">
         <v>235</v>
@@ -4338,340 +4347,324 @@
       <c r="I75" s="6"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="8">
-        <v>26</v>
-      </c>
+      <c r="A76" s="8"/>
       <c r="B76" s="8" t="s">
-        <v>357</v>
+        <v>168</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I76" s="6" t="s">
-        <v>260</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="I76" s="6"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="8">
-        <v>27</v>
-      </c>
+      <c r="A77" s="8"/>
       <c r="B77" s="8" t="s">
-        <v>364</v>
+        <v>172</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I77" s="6" t="s">
-        <v>247</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="I77" s="6"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="8">
-        <v>28</v>
-      </c>
+      <c r="A78" s="8"/>
       <c r="B78" s="8" t="s">
-        <v>365</v>
+        <v>174</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I78" s="6" t="s">
-        <v>247</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="I78" s="6"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="8">
-        <v>29</v>
-      </c>
+      <c r="A79" s="8"/>
       <c r="B79" s="8" t="s">
-        <v>370</v>
+        <v>352</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I79" s="6" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="I79" s="6"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="8" t="s">
-        <v>371</v>
+        <v>353</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>395</v>
+        <v>63</v>
       </c>
       <c r="H80" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I80" s="6"/>
     </row>
-    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
       <c r="B81" s="8" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E81" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="H81" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I81" s="6"/>
     </row>
-    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="8"/>
       <c r="B82" s="8" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>106</v>
+        <v>68</v>
       </c>
       <c r="H82" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I82" s="6"/>
     </row>
-    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="8"/>
       <c r="B83" s="8" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="H83" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I83" s="6"/>
     </row>
-    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="B84" s="8" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="H84" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I84" s="6"/>
     </row>
-    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="8"/>
       <c r="B85" s="8" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="H85" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I85" s="6"/>
     </row>
-    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="8"/>
       <c r="B86" s="8" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H86" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I86" s="6"/>
     </row>
-    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="8"/>
       <c r="B87" s="8" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="H87" s="6" t="s">
         <v>235</v>
       </c>
       <c r="I87" s="6"/>
     </row>
-    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
       <c r="B88" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="H88" s="6" t="s">
         <v>235</v>
@@ -4690,22 +4683,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D533DA-9B44-4E62-8880-E2761E1543A9}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="123.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="114.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="114.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>142</v>
       </c>
@@ -4713,493 +4705,403 @@
         <v>228</v>
       </c>
       <c r="C1" t="s">
-        <v>398</v>
+        <v>229</v>
       </c>
       <c r="D1" t="s">
-        <v>229</v>
+        <v>263</v>
       </c>
       <c r="E1" t="s">
-        <v>263</v>
-      </c>
-      <c r="F1" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>301</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C2" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="D2" s="5" t="b">
+      <c r="C2" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>302</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C3" s="2">
-        <v>3</v>
-      </c>
-      <c r="D3" s="5" t="b">
+      <c r="C3" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>303</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C4" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D4" s="5" t="b">
+      <c r="C4" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>304</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C5" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D5" s="5" t="b">
+      <c r="C5" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>305</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="C6" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D6" s="5" t="b">
+      <c r="C6" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>310</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C7" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D7" s="5" t="b">
+      <c r="C7" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>342</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C8" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D8" s="5" t="b">
+      <c r="C8" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>350</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="C9" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D9" s="5" t="b">
+      <c r="C9" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>356</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C10" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="D10" s="5" t="b">
+      <c r="C10" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>362</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C11" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D11" s="5" t="b">
+      <c r="C11" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>363</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="C12" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="D12" s="5" t="b">
+      <c r="C12" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>367</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C13" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D13" s="5" t="b">
+      <c r="C13" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>368</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C14" s="2">
-        <v>3</v>
-      </c>
-      <c r="D14" s="5" t="b">
+      <c r="C14" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>369</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C15" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="D15" s="5" t="b">
+      <c r="C15" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>316</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C16" s="2">
-        <v>4</v>
-      </c>
-      <c r="D16" s="5" t="b">
+      <c r="C16" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>128</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C17" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D17" s="5" t="b">
+      <c r="C17" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>129</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C18" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D18" s="5" t="b">
+      <c r="C18" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="C19" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D19" s="5" t="b">
+      <c r="C19" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>320</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="C20" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D20" s="5" t="b">
+      <c r="C20" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>321</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="C21" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D21" s="5" t="b">
+      <c r="C21" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>343</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C22" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D22" s="5" t="b">
+      <c r="C22" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>344</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C23" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D23" s="5" t="b">
+      <c r="C23" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>345</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="D24" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>354</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="D25" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>355</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="C26" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D26" s="5" t="b">
+      <c r="C26" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>357</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="C27" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D27" s="5" t="b">
+      <c r="C27" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>364</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="D28" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>365</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="D29" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>370</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="D30" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F30" s="2"/>
+      <c r="E30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5214,7 +5116,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5316,7 +5218,7 @@
         <v>399</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>